<commit_message>
Fix: Excel sheet merge
</commit_message>
<xml_diff>
--- a/1984/Assets/Resources/Story/StoryData.xlsx
+++ b/1984/Assets/Resources/Story/StoryData.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janghyun\Desktop\JangHyun\Programming\Github\1984_Project\1984\Assets\Resources\Dialogue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janghyun\Desktop\JangHyun\Programming\GitHub\1984_Project\1984\Assets\Resources\Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873FA037-D181-4CC7-94B4-20A016448A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0C638-C36E-4F1B-BD7E-5D5DEC8879C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21630" yWindow="5295" windowWidth="20220" windowHeight="13005" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="2988" windowWidth="23040" windowHeight="13596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dialogue" sheetId="1" r:id="rId1"/>
-    <sheet name="Option" sheetId="4" r:id="rId2"/>
-    <sheet name="Character" sheetId="2" r:id="rId3"/>
-    <sheet name="Scene" sheetId="3" r:id="rId4"/>
+    <sheet name="Story" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
-  <si>
-    <t>윈스턴</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>네, 반가워요</t>
   </si>
@@ -65,58 +59,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Art</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>State</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Idle</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Option</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Dialogue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>자고싶어요</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>줄리아</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>사주시려고요?</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Description</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Julia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crying</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting</t>
-  </si>
-  <si>
-    <t>FirstMeeting</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -125,14 +84,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>첫 만남</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Winston</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -141,51 +92,30 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>OtherScene</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-1-2 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-1-1 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-0-3 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-0-1 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-0-2 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstMeeting-1-3 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OtherScene-0-1 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OtherScene-0-2 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OtherScene-1-1 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OtherScene-1-2 선택지</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>임시 장면</t>
+    <t>Goto</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t>. . . .</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>식사 하셨나요?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>피곤하시죠?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>그냥 갈게요,,</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1162,535 +1092,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.8984375" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02807097-E48C-467E-A26B-410FD7F4E95A}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F908B675-3897-4B22-94B9-79BB7E37ACE2}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f>CONCATENATE(A2,C2)</f>
-        <v>WinstonIdle</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f t="shared" ref="D3:D57" si="0">CONCATENATE(A3,C3)</f>
-        <v>WinstonCrying</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>JuliaIdle</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54489F72-A99A-4889-8CCE-D2CE6F7C2670}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="48.125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Dialogue Active 헤더 추가
+ 등장인물 발언 시 이미지 활성화
+ Active 헤더로 대화중 등장인물 사라짐 구분
+ 버튼 선택시 해당 대화 출력
</commit_message>
<xml_diff>
--- a/1984/Assets/Resources/Story/StoryData.xlsx
+++ b/1984/Assets/Resources/Story/StoryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janghyun\Desktop\JangHyun\Programming\GitHub\1984_Project\1984\Assets\Resources\Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F94846-32D5-4EDF-B848-E6FAD8933409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA5A843-7950-4874-A1C7-567BB15EC65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1608" yWindow="348" windowWidth="23040" windowHeight="13596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>네, 반가워요</t>
   </si>
@@ -99,10 +99,6 @@
     <t>Dialogue</t>
   </si>
   <si>
-    <t>. . . .</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>식사 하셨나요?</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -124,6 +120,18 @@
   </si>
   <si>
     <t>InRoom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>나래이션 양식</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>독백, 방백 양식</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1100,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1115,10 +1123,11 @@
     <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.8984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="9" style="2"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1138,10 +1147,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1152,16 +1164,16 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1172,16 +1184,16 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -1195,16 +1207,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -1218,16 +1230,16 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -1241,16 +1253,16 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1261,16 +1273,16 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1284,16 +1296,19 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1304,16 +1319,16 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1327,16 +1342,19 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1350,16 +1368,19 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -1370,33 +1391,30 @@
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>